<commit_message>
results of bert for laptop on 0% latency
</commit_message>
<xml_diff>
--- a/output/SemEval-14/Laptop/agg.pred.eval.mean.10.0.0.xlsx
+++ b/output/SemEval-14/Laptop/agg.pred.eval.mean.10.0.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farinam\PycharmProjects\LADy\output\SemEval-14\Laptop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Github\Fani-Lab\lady\main\output\SemEval-14\Laptop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58DE42E-5C84-4576-8C86-C85E5959EFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C44CC6-31A6-41D2-80A6-048F1ABA09DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="21210" windowHeight="12990" activeTab="2" xr2:uid="{53722CFA-7A49-4FF3-BDD5-F566020460F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{53722CFA-7A49-4FF3-BDD5-F566020460F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -877,7 +877,48 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -19790,8 +19831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEAE7E8B-6D93-4171-9A24-226920DB92D8}">
   <dimension ref="A1:AG10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AD11" sqref="AD11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AD3" sqref="AD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20042,16 +20083,16 @@
       <c r="AC3" s="30">
         <v>0.53382550335570467</v>
       </c>
-      <c r="AD3" s="2">
+      <c r="AD3" s="19">
         <v>0.61935483870967745</v>
       </c>
-      <c r="AE3" s="2">
+      <c r="AE3" s="19">
         <v>0.64865262233925836</v>
       </c>
-      <c r="AF3" s="2">
+      <c r="AF3" s="19">
         <v>0.62346939903204812</v>
       </c>
-      <c r="AG3" s="2">
+      <c r="AG3" s="19">
         <v>0.56712307073366985</v>
       </c>
     </row>
@@ -20143,16 +20184,16 @@
       <c r="AC4" s="25">
         <v>0.59167785234899328</v>
       </c>
-      <c r="AD4" s="2">
+      <c r="AD4" s="3">
         <v>0.60184331797235013</v>
       </c>
-      <c r="AE4" s="2">
+      <c r="AE4" s="16">
         <v>0.63472350230414742</v>
       </c>
-      <c r="AF4" s="2">
+      <c r="AF4" s="3">
         <v>0.61015886297909738</v>
       </c>
-      <c r="AG4" s="2">
+      <c r="AG4" s="3">
         <v>0.5526340428644575</v>
       </c>
     </row>
@@ -20244,16 +20285,16 @@
       <c r="AC5" s="16">
         <v>0.59178970917225948</v>
       </c>
-      <c r="AD5" s="2">
+      <c r="AD5" s="3">
         <v>0.60737327188940093</v>
       </c>
-      <c r="AE5" s="2">
+      <c r="AE5" s="3">
         <v>0.63142857142857145</v>
       </c>
-      <c r="AF5" s="2">
+      <c r="AF5" s="3">
         <v>0.60921670361655456</v>
       </c>
-      <c r="AG5" s="2">
+      <c r="AG5" s="3">
         <v>0.55329260844122585</v>
       </c>
     </row>
@@ -20345,16 +20386,16 @@
       <c r="AC6" s="3">
         <v>0.57599552572706947</v>
       </c>
-      <c r="AD6" s="2">
+      <c r="AD6" s="3">
         <v>0.60184331797235013</v>
       </c>
-      <c r="AE6" s="2">
+      <c r="AE6" s="3">
         <v>0.6237173579109061</v>
       </c>
-      <c r="AF6" s="2">
+      <c r="AF6" s="3">
         <v>0.60387398727080899</v>
       </c>
-      <c r="AG6" s="2">
+      <c r="AG6" s="3">
         <v>0.54852680857289149</v>
       </c>
     </row>
@@ -20446,16 +20487,16 @@
       <c r="AC7" s="3">
         <v>0.58194630872483222</v>
       </c>
-      <c r="AD7" s="2">
+      <c r="AD7" s="16">
         <v>0.61843317972350231</v>
       </c>
-      <c r="AE7" s="2">
+      <c r="AE7" s="3">
         <v>0.62901689708141317</v>
       </c>
-      <c r="AF7" s="2">
+      <c r="AF7" s="16">
         <v>0.61122936171134368</v>
       </c>
-      <c r="AG7" s="2">
+      <c r="AG7" s="16">
         <v>0.55606427839953176</v>
       </c>
     </row>
@@ -20547,16 +20588,16 @@
       <c r="AC8" s="3">
         <v>0.59035794183445189</v>
       </c>
-      <c r="AD8" s="2">
+      <c r="AD8" s="3">
         <v>0.60552995391705067</v>
       </c>
-      <c r="AE8" s="2">
+      <c r="AE8" s="3">
         <v>0.63361531709457974</v>
       </c>
-      <c r="AF8" s="2">
+      <c r="AF8" s="3">
         <v>0.60959800209431514</v>
       </c>
-      <c r="AG8" s="2">
+      <c r="AG8" s="3">
         <v>0.55260794748006725</v>
       </c>
     </row>
@@ -20648,16 +20689,16 @@
       <c r="AC9" s="19">
         <v>0.59281879194630882</v>
       </c>
-      <c r="AD9" s="2">
+      <c r="AD9" s="3">
         <v>0.60184331797235024</v>
       </c>
-      <c r="AE9" s="2">
+      <c r="AE9" s="3">
         <v>0.6290520078999341</v>
       </c>
-      <c r="AF9" s="2">
+      <c r="AF9" s="3">
         <v>0.60920417989958642</v>
       </c>
-      <c r="AG9" s="2">
+      <c r="AG9" s="3">
         <v>0.55478922536756636</v>
       </c>
     </row>
@@ -20749,16 +20790,16 @@
       <c r="AC10" s="6">
         <v>0.57787472035794185</v>
       </c>
-      <c r="AD10" s="2">
+      <c r="AD10" s="3">
         <v>0.60276497695852527</v>
       </c>
-      <c r="AE10" s="2">
+      <c r="AE10" s="3">
         <v>0.61943932411674352</v>
       </c>
-      <c r="AF10" s="2">
+      <c r="AF10" s="3">
         <v>0.60248234736646322</v>
       </c>
-      <c r="AG10" s="2">
+      <c r="AG10" s="3">
         <v>0.54630731109648167</v>
       </c>
     </row>
@@ -20775,7 +20816,7 @@
     <mergeCell ref="R1:U1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B10">
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20785,7 +20826,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:AC9 B4:AC4">
-    <cfRule type="colorScale" priority="629">
+    <cfRule type="colorScale" priority="633">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20795,7 +20836,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:AC10 B5:AC8 B3:AC3">
-    <cfRule type="colorScale" priority="895">
+    <cfRule type="colorScale" priority="899">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20805,7 +20846,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C10">
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20815,7 +20856,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D10">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20825,7 +20866,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E10">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20835,7 +20876,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F10">
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20845,7 +20886,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G10">
-    <cfRule type="colorScale" priority="27">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20855,7 +20896,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H10">
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20865,7 +20906,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I10">
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20875,7 +20916,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J10">
-    <cfRule type="colorScale" priority="24">
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20885,7 +20926,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K10">
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20895,7 +20936,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L10">
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20905,7 +20946,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M10">
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20915,7 +20956,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N10">
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20925,7 +20966,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O10">
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20935,7 +20976,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P10">
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20945,7 +20986,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q10">
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20955,7 +20996,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:R10">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20965,7 +21006,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:S10">
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20975,7 +21016,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3:T10">
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20985,7 +21026,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3:U10">
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -20995,7 +21036,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:V10">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -21005,7 +21046,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W3:W10">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -21015,7 +21056,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X3:X10">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -21025,7 +21066,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y3:Y10">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -21035,7 +21076,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z3:Z10">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -21045,7 +21086,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA3:AA10">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -21055,7 +21096,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB3:AB10">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -21065,7 +21106,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC3:AC10">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -21074,6 +21115,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="AD3:AD10">
+    <cfRule type="top10" dxfId="3" priority="4" rank="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE3:AE10">
+    <cfRule type="top10" dxfId="2" priority="3" rank="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF3:AF10">
+    <cfRule type="top10" dxfId="1" priority="2" rank="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG3:AG10">
+    <cfRule type="top10" dxfId="0" priority="1" rank="2"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>